<commit_message>
Implemented upload document functionality.
</commit_message>
<xml_diff>
--- a/docs/db_design.xlsx
+++ b/docs/db_design.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
   <si>
     <t>Sr.No</t>
   </si>
@@ -74,36 +74,24 @@
     <t>state</t>
   </si>
   <si>
-    <t>Emergency Contact</t>
-  </si>
-  <si>
     <t>mobile:string</t>
   </si>
   <si>
     <t>country</t>
   </si>
   <si>
-    <t>Bank Account Information</t>
-  </si>
-  <si>
     <t>address:Foreign key</t>
   </si>
   <si>
     <t>zip code</t>
   </si>
   <si>
-    <t>Tax Information</t>
-  </si>
-  <si>
     <t>skype_id:string</t>
   </si>
   <si>
     <t>department:string</t>
   </si>
   <si>
-    <t>javascript:void(0);</t>
-  </si>
-  <si>
     <t>designation:string</t>
   </si>
   <si>
@@ -140,6 +128,9 @@
     <t>created_at:datetime</t>
   </si>
   <si>
+    <t>Referral</t>
+  </si>
+  <si>
     <t>Client</t>
   </si>
   <si>
@@ -152,6 +143,12 @@
     <t>status: A/I/D</t>
   </si>
   <si>
+    <t>Is_employee:Boolean</t>
+  </si>
+  <si>
+    <t>Define referral is employee or external person</t>
+  </si>
+  <si>
     <t>Project</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
     <t>Employee: foreign key</t>
   </si>
   <si>
+    <t>Referral:Foreign key null true</t>
+  </si>
+  <si>
     <t>Project: foreign key</t>
   </si>
   <si>
@@ -264,6 +264,18 @@
   </si>
   <si>
     <t>qantity</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>organization name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>contact person</t>
   </si>
 </sst>
 </file>
@@ -416,10 +428,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -513,103 +525,103 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="F13" s="0" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,45 +629,69 @@
         <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="F27" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>4</v>
@@ -671,37 +707,37 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>4</v>
@@ -717,110 +753,115 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="7" t="s">
+    <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="7" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B59" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D66" s="0" t="s">
         <v>68</v>
       </c>
     </row>
@@ -872,7 +913,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,10 +950,63 @@
         <v>82</v>
       </c>
     </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I15" r:id="rId1" display="javascript:void(0);"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Created APIs and UI templates for vendor.
</commit_message>
<xml_diff>
--- a/docs/db_design.xlsx
+++ b/docs/db_design.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Sr.No</t>
   </si>
@@ -128,154 +128,109 @@
     <t>created_at:datetime</t>
   </si>
   <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>name: string</t>
+  </si>
+  <si>
+    <t>phone:string</t>
+  </si>
+  <si>
+    <t>status: A/I/D</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>description:textarea</t>
+  </si>
+  <si>
+    <t>owner: foreign key(client)</t>
+  </si>
+  <si>
+    <t>representative:foreign key(employee)</t>
+  </si>
+  <si>
+    <t>status: A/I/C/D</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Employee: foreign key</t>
+  </si>
+  <si>
+    <t>Referral:Foreign key null true</t>
+  </si>
+  <si>
+    <t>Project: foreign key</t>
+  </si>
+  <si>
+    <t>role: string</t>
+  </si>
+  <si>
+    <t>start_date: date</t>
+  </si>
+  <si>
+    <t>end_date: date</t>
+  </si>
+  <si>
+    <t>duration_per_day:integer(seconds)</t>
+  </si>
+  <si>
+    <t>pay_rate_type</t>
+  </si>
+  <si>
+    <t>pay_rate: float</t>
+  </si>
+  <si>
+    <t>billing_cycle:weekly/bi-weekly/monthly</t>
+  </si>
+  <si>
+    <t>Remark:string</t>
+  </si>
+  <si>
+    <t>timesheet</t>
+  </si>
+  <si>
+    <t>contract:foreign_key</t>
+  </si>
+  <si>
+    <t>sign_in: datetimne</t>
+  </si>
+  <si>
+    <t>sign_out: datetime</t>
+  </si>
+  <si>
+    <t>completed_tasks_description: textarea</t>
+  </si>
+  <si>
+    <t>is_billable:boolean</t>
+  </si>
+  <si>
+    <t>status:P/A/R/D</t>
+  </si>
+  <si>
+    <t>Pending/Approved/Rejected/Delete</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>organization name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>contact person</t>
+  </si>
+  <si>
     <t>Referral</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>name: string</t>
-  </si>
-  <si>
-    <t>phone:string</t>
-  </si>
-  <si>
-    <t>status: A/I/D</t>
-  </si>
-  <si>
-    <t>Is_employee:Boolean</t>
-  </si>
-  <si>
-    <t>Define referral is employee or external person</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>description:textarea</t>
-  </si>
-  <si>
-    <t>owner: foreign key(client)</t>
-  </si>
-  <si>
-    <t>representative:foreign key(employee)</t>
-  </si>
-  <si>
-    <t>status: A/I/C/D</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Employee: foreign key</t>
-  </si>
-  <si>
-    <t>Referral:Foreign key null true</t>
-  </si>
-  <si>
-    <t>Project: foreign key</t>
-  </si>
-  <si>
-    <t>role: string</t>
-  </si>
-  <si>
-    <t>start_date: date</t>
-  </si>
-  <si>
-    <t>end_date: date</t>
-  </si>
-  <si>
-    <t>duration_per_day:integer(seconds)</t>
-  </si>
-  <si>
-    <t>pay_rate_type</t>
-  </si>
-  <si>
-    <t>pay_rate: float</t>
-  </si>
-  <si>
-    <t>billing_cycle:weekly/bi-weekly/monthly</t>
-  </si>
-  <si>
-    <t>Remark:string</t>
-  </si>
-  <si>
-    <t>timesheet</t>
-  </si>
-  <si>
-    <t>contract:foreign_key</t>
-  </si>
-  <si>
-    <t>sign_in: datetimne</t>
-  </si>
-  <si>
-    <t>sign_out: datetime</t>
-  </si>
-  <si>
-    <t>completed_tasks_description: textarea</t>
-  </si>
-  <si>
-    <t>is_billable:boolean</t>
-  </si>
-  <si>
-    <t>status:P/A/R/D</t>
-  </si>
-  <si>
-    <t>Pending/Approved/Rejected/Delete</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>due date</t>
-  </si>
-  <si>
-    <t>many to many services</t>
-  </si>
-  <si>
-    <t>tax:decimal</t>
-  </si>
-  <si>
-    <t>total_amount:decimal</t>
-  </si>
-  <si>
-    <t>discount:decimal</t>
-  </si>
-  <si>
-    <t>Remark:textarea</t>
-  </si>
-  <si>
-    <t>status: P/U/D</t>
-  </si>
-  <si>
-    <t>Paid/Unpaid/Delete</t>
-  </si>
-  <si>
-    <t>Invoice_items</t>
-  </si>
-  <si>
-    <t>service_name: string</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>qantity</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
-    <t>organization name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>contact person</t>
+    <t>employee: foreign key</t>
   </si>
 </sst>
 </file>
@@ -428,10 +383,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C93" activeCellId="0" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -616,77 +571,45 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,7 +622,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>4</v>
@@ -707,22 +630,22 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +655,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>4</v>
@@ -753,62 +676,62 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>4</v>
@@ -829,27 +752,27 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,151 +782,112 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B68" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="0" t="s">
+      <c r="B69" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" s="0" t="s">
+      <c r="B80" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
-        <v>82</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B85" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="C85" s="0" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="0" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created user with assigned role after employee successfully saved.
</commit_message>
<xml_diff>
--- a/docs/db_design.xlsx
+++ b/docs/db_design.xlsx
@@ -5,352 +5,350 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="963" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Tracker" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
-  <si>
-    <t xml:space="preserve">Sr.No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attributes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id: primary key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auth user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is_manager:boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True: Manger/ False: others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first_name: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employee_id:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address:Foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joined Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skype_id:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">department:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">designation:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emp_type:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Pay rate type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hourly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Pay rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$ 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passport_no:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Visa Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H-1B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">referral_bonus_points: Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emergency_contact: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bank_account_info: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_info: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">document: file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status: A/U/D/V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Available/Unavailable/Delete/Vacation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">created_at:datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status: A/I/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active/Inactive/Delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vendor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">organization name: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact person: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employee: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line1: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line2: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city/village: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zip code: PositiveInteger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EmergencyContact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relation: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BankAccountInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bank_name: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bank_routing_no: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">account_no: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">account_type: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TaxInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filling_status:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single/Joint/Exempt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">withholding_allowance: float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_withholding: float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_withholding_declare: boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">representative: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start_date: date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_date: date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duration_per_day:integer(seconds)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pay_rate_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pay_rate: float</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billing_cycle:weekly/bi-weekly/monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referral:Foreign key null true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status: I/C/O/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inprogress/Complete/Onhold/Delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description:textarea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">located_at:Foreign key(Address)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">owner: foreign key(client)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_members:many_to_many(employee)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activites: many to many(ProjectActivity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProjectActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timesheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contract:foreign_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sign_in: datetimne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sign_out: datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status:I/P/A/R/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pending/Approved/Rejected/Delete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TimesheetTask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timesheet: foreign key(Timesheet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start_time: datetimne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_time: datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activity: foreign key(ProjectActivity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity belong to selected project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note: string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_billable:boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assignment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emp: foreign key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">due_date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="111">
+  <si>
+    <t>Sr.No</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>id: primary key</t>
+  </si>
+  <si>
+    <t>Auth user</t>
+  </si>
+  <si>
+    <t>username: string</t>
+  </si>
+  <si>
+    <t>password: string</t>
+  </si>
+  <si>
+    <t>email: string</t>
+  </si>
+  <si>
+    <t>Is_manager:boolean</t>
+  </si>
+  <si>
+    <t>True: Manger/ False: others</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>first_name: string</t>
+  </si>
+  <si>
+    <t>last_name: string</t>
+  </si>
+  <si>
+    <t>employee_id:string</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>gender:string</t>
+  </si>
+  <si>
+    <t>address:Foreign key</t>
+  </si>
+  <si>
+    <t>Joined Date</t>
+  </si>
+  <si>
+    <t>mobile:string</t>
+  </si>
+  <si>
+    <t>skype_id:string</t>
+  </si>
+  <si>
+    <t>department:string</t>
+  </si>
+  <si>
+    <t>designation:string</t>
+  </si>
+  <si>
+    <t>emp_type:string</t>
+  </si>
+  <si>
+    <t>Current Pay rate type</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>Current Pay rate</t>
+  </si>
+  <si>
+    <t>$ 10</t>
+  </si>
+  <si>
+    <t>passport_no:string</t>
+  </si>
+  <si>
+    <t>Current Visa Status</t>
+  </si>
+  <si>
+    <t>H-1B</t>
+  </si>
+  <si>
+    <t>referral_bonus_points: Integer</t>
+  </si>
+  <si>
+    <t>emergency_contact: foreign key</t>
+  </si>
+  <si>
+    <t>bank_account_info: foreign key</t>
+  </si>
+  <si>
+    <t>tax_info: foreign key</t>
+  </si>
+  <si>
+    <t>document: file</t>
+  </si>
+  <si>
+    <t>status: A/U/D/V</t>
+  </si>
+  <si>
+    <t>Available/Unavailable/Delete/Vacation</t>
+  </si>
+  <si>
+    <t>created_at:datetime</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>status: A/I/D</t>
+  </si>
+  <si>
+    <t>Active/Inactive/Delete</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>organization name: string</t>
+  </si>
+  <si>
+    <t>contact person: string</t>
+  </si>
+  <si>
+    <t>Remark:string</t>
+  </si>
+  <si>
+    <t>Referral</t>
+  </si>
+  <si>
+    <t>employee: foreign key</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>line1: string</t>
+  </si>
+  <si>
+    <t>line2: string</t>
+  </si>
+  <si>
+    <t>city/village: string</t>
+  </si>
+  <si>
+    <t>state: string</t>
+  </si>
+  <si>
+    <t>country: string</t>
+  </si>
+  <si>
+    <t>zip code: PositiveInteger</t>
+  </si>
+  <si>
+    <t>EmergencyContact</t>
+  </si>
+  <si>
+    <t>relation: string</t>
+  </si>
+  <si>
+    <t>BankAccountInfo</t>
+  </si>
+  <si>
+    <t>bank_name: string</t>
+  </si>
+  <si>
+    <t>bank_routing_no: string</t>
+  </si>
+  <si>
+    <t>account_no: string</t>
+  </si>
+  <si>
+    <t>account_type: string</t>
+  </si>
+  <si>
+    <t>TaxInfo</t>
+  </si>
+  <si>
+    <t>filling_status:string</t>
+  </si>
+  <si>
+    <t>Single/Joint/Exempt</t>
+  </si>
+  <si>
+    <t>withholding_allowance: float</t>
+  </si>
+  <si>
+    <t>additional_withholding: float</t>
+  </si>
+  <si>
+    <t>is_withholding_declare: boolean</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>representative: foreign key</t>
+  </si>
+  <si>
+    <t>Client: foreign key</t>
+  </si>
+  <si>
+    <t>Employee: foreign key</t>
+  </si>
+  <si>
+    <t>role: string</t>
+  </si>
+  <si>
+    <t>start_date: date</t>
+  </si>
+  <si>
+    <t>end_date: date</t>
+  </si>
+  <si>
+    <t>duration_per_day:integer(seconds)</t>
+  </si>
+  <si>
+    <t>pay_rate_type</t>
+  </si>
+  <si>
+    <t>pay_rate: float</t>
+  </si>
+  <si>
+    <t>billing_cycle:weekly/bi-weekly/monthly</t>
+  </si>
+  <si>
+    <t>Referral:Foreign key null true</t>
+  </si>
+  <si>
+    <t>status: I/C/O/D</t>
+  </si>
+  <si>
+    <t>Inprogress/Complete/Onhold/Delete</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>name: string</t>
+  </si>
+  <si>
+    <t>description:textarea</t>
+  </si>
+  <si>
+    <t>located_at:Foreign key(Address)</t>
+  </si>
+  <si>
+    <t>owner: foreign key(client)</t>
+  </si>
+  <si>
+    <t>project_members:many_to_many(employee)</t>
+  </si>
+  <si>
+    <t>activites: many to many(ProjectActivity)</t>
+  </si>
+  <si>
+    <t>ProjectActivity</t>
+  </si>
+  <si>
+    <t>name:string</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>contract:foreign_key</t>
+  </si>
+  <si>
+    <t>sign_in: datetimne</t>
+  </si>
+  <si>
+    <t>sign_out: datetime</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>status:I/P/A/R/D</t>
+  </si>
+  <si>
+    <t>Pending/Approved/Rejected/Delete</t>
+  </si>
+  <si>
+    <t>TimesheetTask</t>
+  </si>
+  <si>
+    <t>timesheet: foreign key(Timesheet)</t>
+  </si>
+  <si>
+    <t>start_time: datetimne</t>
+  </si>
+  <si>
+    <t>end_time: datetime</t>
+  </si>
+  <si>
+    <t>Project: foreign key</t>
+  </si>
+  <si>
+    <t>activity: foreign key(ProjectActivity)</t>
+  </si>
+  <si>
+    <t>Activity belong to selected project</t>
+  </si>
+  <si>
+    <t>note: string</t>
+  </si>
+  <si>
+    <t>is_billable:boolean</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Emp: foreign key</t>
+  </si>
+  <si>
+    <t>due_date</t>
   </si>
 </sst>
 </file>
@@ -358,7 +356,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1072,15 +1070,17 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1296,12 +1296,17 @@
       <c r="C38" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1310,7 +1315,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>5</v>
@@ -1318,40 +1323,40 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,7 +1364,7 @@
         <v>6</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>5</v>
@@ -1367,22 +1372,22 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>